<commit_message>
Some fixed to equations!
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A5D1AF-B594-ED42-8E42-7ECF5BBB3683}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6091AE-EE47-5046-B1DE-D53C164C1A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20240" yWindow="740" windowWidth="10000" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
+    <workbookView xWindow="17820" yWindow="740" windowWidth="12420" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zezza import" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="914">
   <si>
     <t>wfcreate berlin u 1 200</t>
   </si>
@@ -3228,13 +3228,10 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59908B7B-EBC3-344F-9113-3BA63F6E78FB}" name="Tabelle1" displayName="Tabelle1" ref="A1:D138" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Housing Market"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
+    <sortCondition ref="B1:B138"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7F596A33-4614-6C40-BB1D-09C449AA6172}" name="Number" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{40BBDBA3-8B58-3F49-902D-6228A1A56631}" name="Sector" dataDxfId="1"/>
@@ -5750,6 +5747,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5946,6 +5944,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5953,8 +5952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="C106" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5987,7 +5986,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5998,232 +5997,238 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2</v>
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>3</v>
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>9</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46">
-        <v>4</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>878</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>32</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>745</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>424</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>37</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>421</v>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>41</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46">
-        <v>8</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>878</v>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>42</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>745</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>743</v>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>51</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>423</v>
+        <v>475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>52</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46">
-        <v>12</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>878</v>
+        <v>476</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>53</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>424</v>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>67</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>14</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>421</v>
+        <v>489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>90</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>421</v>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>91</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46">
-        <v>16</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>878</v>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>113</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46">
-        <v>17</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>878</v>
+        <v>534</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>120</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>745</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>424</v>
+        <v>894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>121</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>745</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>19</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>421</v>
+        <v>895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>424</v>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>39</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>21</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>421</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>40</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
-        <v>22</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>423</v>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>112</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6234,7 +6239,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6245,1199 +6250,1235 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>25</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>743</v>
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>99</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>423</v>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>103</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8">
-        <v>27</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>423</v>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>106</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8">
-        <v>28</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>423</v>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>114</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>423</v>
+        <v>535</v>
+      </c>
+      <c r="D29" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>115</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>453</v>
+        <v>536</v>
       </c>
       <c r="D30" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8">
-        <v>30</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>423</v>
+        <v>911</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>116</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>454</v>
+        <v>537</v>
       </c>
       <c r="D31" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8">
-        <v>31</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>423</v>
+        <v>912</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>123</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
-        <v>32</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
-        <v>33</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>124</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>125</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>126</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>127</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
+        <v>6</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
+        <v>13</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
+        <v>18</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
+        <v>20</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B41" s="15" t="s">
         <v>424</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C41" s="13" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+    <row r="42" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B42" s="15" t="s">
         <v>424</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C42" s="13" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6">
-        <v>36</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>37</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <v>38</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <v>39</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <v>40</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
-        <v>41</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
-        <v>42</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>745</v>
+    <row r="43" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
+        <v>43</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>424</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>44</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
+        <v>61</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
-        <v>45</v>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
+        <v>68</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>424</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
-        <v>47</v>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
+        <v>93</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
-        <v>48</v>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
+        <v>94</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="8">
-        <v>49</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>423</v>
+        <v>516</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
+        <v>95</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
-        <v>50</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>745</v>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
+        <v>96</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
-        <v>51</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>745</v>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
+        <v>100</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
-        <v>52</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>745</v>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
+        <v>107</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
-        <v>53</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>745</v>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
+        <v>108</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>54</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>743</v>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
+        <v>109</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>55</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>743</v>
+        <v>530</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
+        <v>117</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="7">
-        <v>56</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>743</v>
+        <v>538</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="10">
+        <v>72</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="7">
-        <v>57</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>743</v>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="10">
+        <v>73</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="7">
-        <v>58</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>743</v>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10">
+        <v>74</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="8">
-        <v>59</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>423</v>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="10">
+        <v>75</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="46">
-        <v>60</v>
-      </c>
-      <c r="B61" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
-        <v>61</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>424</v>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="10">
+        <v>76</v>
+      </c>
+      <c r="B61" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="10">
+        <v>77</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="6">
-        <v>62</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C63" s="45" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="46">
-        <v>63</v>
-      </c>
-      <c r="B64" s="47" t="s">
-        <v>878</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="10">
+        <v>78</v>
+      </c>
+      <c r="B63" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="10">
+        <v>79</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="8">
-        <v>64</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>423</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="10">
+        <v>80</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C65" s="13" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="8">
-        <v>65</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>423</v>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="10">
+        <v>81</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="7">
-        <v>66</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>743</v>
+        <v>503</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="10">
+        <v>82</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C67" s="13" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
-        <v>67</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>745</v>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="10">
+        <v>83</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C68" s="13" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="5">
-        <v>68</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>424</v>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="10">
+        <v>84</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="6">
-        <v>69</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>421</v>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="10">
+        <v>85</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="5">
-        <v>70</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>424</v>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="10">
+        <v>86</v>
+      </c>
+      <c r="B71" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="6">
-        <v>71</v>
-      </c>
-      <c r="B72" s="16" t="s">
-        <v>421</v>
+        <v>508</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="10">
+        <v>87</v>
+      </c>
+      <c r="B72" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C72" s="13" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="10">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="10">
-        <v>80</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>746</v>
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="46">
+        <v>118</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>878</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="10">
-        <v>82</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>746</v>
+        <v>540</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>11</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="10">
-        <v>83</v>
-      </c>
-      <c r="B84" s="20" t="s">
-        <v>746</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="8">
+        <v>22</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="10">
-        <v>84</v>
-      </c>
-      <c r="B85" s="20" t="s">
-        <v>746</v>
+        <v>446</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="8">
+        <v>26</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="10">
-        <v>85</v>
-      </c>
-      <c r="B86" s="20" t="s">
-        <v>746</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="8">
+        <v>27</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="10">
-        <v>86</v>
-      </c>
-      <c r="B87" s="20" t="s">
-        <v>746</v>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8">
+        <v>28</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="10">
-        <v>87</v>
-      </c>
-      <c r="B88" s="20" t="s">
-        <v>746</v>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="8">
+        <v>29</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="10">
-        <v>88</v>
-      </c>
-      <c r="B89" s="20" t="s">
-        <v>746</v>
+        <v>453</v>
+      </c>
+      <c r="D88" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="8">
+        <v>30</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="10">
-        <v>89</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>746</v>
+        <v>454</v>
+      </c>
+      <c r="D89" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="8">
+        <v>31</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="4">
-        <v>90</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>745</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="8">
+        <v>49</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C91" s="13" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="4">
-        <v>91</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>745</v>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="8">
+        <v>59</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="7">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="8">
+        <v>64</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="8">
+        <v>65</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="8">
+        <v>104</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="8">
+        <v>105</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>122</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="D97" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="7">
+        <v>10</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="7">
+        <v>25</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="7">
+        <v>54</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="7">
+        <v>55</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="7">
+        <v>56</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="7">
+        <v>57</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="7">
+        <v>58</v>
+      </c>
+      <c r="B104" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="7">
+        <v>66</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="7">
         <v>92</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B106" s="17" t="s">
         <v>743</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C106" s="13" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="5">
-        <v>93</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="5">
-        <v>94</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C95" s="13" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="5">
-        <v>95</v>
-      </c>
-      <c r="B96" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="5">
-        <v>96</v>
-      </c>
-      <c r="B97" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="6">
-        <v>98</v>
-      </c>
-      <c r="B98" s="16" t="s">
+    <row r="107" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="12">
+        <v>129</v>
+      </c>
+      <c r="B107" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="12">
+        <v>130</v>
+      </c>
+      <c r="B108" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="12">
+        <v>131</v>
+      </c>
+      <c r="B109" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="12">
+        <v>132</v>
+      </c>
+      <c r="B110" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="12">
+        <v>133</v>
+      </c>
+      <c r="B111" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="12">
+        <v>134</v>
+      </c>
+      <c r="B112" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="12">
+        <v>135</v>
+      </c>
+      <c r="B113" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="12">
+        <v>2</v>
+      </c>
+      <c r="B114" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="12">
+        <v>3</v>
+      </c>
+      <c r="B115" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="46">
+        <v>4</v>
+      </c>
+      <c r="B116" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="46">
+        <v>8</v>
+      </c>
+      <c r="B117" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="46">
+        <v>12</v>
+      </c>
+      <c r="B118" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="46">
+        <v>16</v>
+      </c>
+      <c r="B119" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C119" s="13" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="46">
+        <v>17</v>
+      </c>
+      <c r="B120" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="46">
+        <v>60</v>
+      </c>
+      <c r="B121" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C121" s="23" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="46">
+        <v>63</v>
+      </c>
+      <c r="B122" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="46">
+        <v>102</v>
+      </c>
+      <c r="B123" s="47" t="s">
+        <v>878</v>
+      </c>
+      <c r="C123" s="13" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="6">
+        <v>7</v>
+      </c>
+      <c r="B124" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="C98" s="13" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="9">
-        <v>99</v>
-      </c>
-      <c r="B99" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C99" s="13" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="5">
-        <v>100</v>
-      </c>
-      <c r="B100" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="6">
-        <v>101</v>
-      </c>
-      <c r="B101" s="16" t="s">
+      <c r="C124" s="13" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="6">
+        <v>14</v>
+      </c>
+      <c r="B125" s="16" t="s">
         <v>421</v>
       </c>
-      <c r="C101" s="13" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="46">
-        <v>102</v>
-      </c>
-      <c r="B102" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="9">
-        <v>103</v>
-      </c>
-      <c r="B103" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="8">
-        <v>104</v>
-      </c>
-      <c r="B104" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="8">
-        <v>105</v>
-      </c>
-      <c r="B105" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="9">
-        <v>106</v>
-      </c>
-      <c r="B106" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="5">
-        <v>107</v>
-      </c>
-      <c r="B107" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="5">
-        <v>108</v>
-      </c>
-      <c r="B108" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="5">
-        <v>109</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="3">
-        <v>110</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="3">
-        <v>111</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="3">
-        <v>112</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4">
-        <v>113</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="9">
-        <v>114</v>
-      </c>
-      <c r="B114" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>535</v>
-      </c>
-      <c r="D114" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="9">
-        <v>115</v>
-      </c>
-      <c r="B115" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>536</v>
-      </c>
-      <c r="D115" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="9">
-        <v>116</v>
-      </c>
-      <c r="B116" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>537</v>
-      </c>
-      <c r="D116" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="5">
-        <v>117</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C117" s="13" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="3">
-        <v>118</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="3">
-        <v>119</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="11">
-        <v>120</v>
-      </c>
-      <c r="B120" s="21" t="s">
-        <v>745</v>
-      </c>
-      <c r="C120" s="13" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="11">
-        <v>121</v>
-      </c>
-      <c r="B121" s="21" t="s">
-        <v>745</v>
-      </c>
-      <c r="C121" s="13" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="8">
-        <v>122</v>
-      </c>
-      <c r="B122" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C122" s="13" t="s">
-        <v>541</v>
-      </c>
-      <c r="D122" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="9">
-        <v>123</v>
-      </c>
-      <c r="B123" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C123" s="13" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="9">
-        <v>124</v>
-      </c>
-      <c r="B124" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C124" s="23" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="9">
-        <v>125</v>
-      </c>
-      <c r="B125" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C125" s="23" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="9">
-        <v>126</v>
-      </c>
-      <c r="B126" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C126" s="23" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="9">
-        <v>127</v>
-      </c>
-      <c r="B127" s="19" t="s">
-        <v>422</v>
+      <c r="C125" s="13" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="6">
+        <v>15</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C126" s="13" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="6">
+        <v>19</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
-        <v>128</v>
+        <v>21</v>
       </c>
       <c r="B128" s="16" t="s">
         <v>421</v>
       </c>
       <c r="C128" s="13" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="6">
+        <v>36</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="6">
+        <v>62</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C130" s="45" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="6">
+        <v>69</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C131" s="13" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="6">
+        <v>71</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C132" s="13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="6">
+        <v>98</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="6">
+        <v>101</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="6">
+        <v>128</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C135" s="13" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="12">
-        <v>129</v>
-      </c>
-      <c r="B129" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C129" s="13" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="12">
-        <v>130</v>
-      </c>
-      <c r="B130" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C130" s="13" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="12">
-        <v>131</v>
-      </c>
-      <c r="B131" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C131" s="13" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="12">
-        <v>132</v>
-      </c>
-      <c r="B132" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C132" s="13" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="12">
-        <v>133</v>
-      </c>
-      <c r="B133" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C133" s="13" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="12">
-        <v>134</v>
-      </c>
-      <c r="B134" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C134" s="13" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="12">
-        <v>135</v>
-      </c>
-      <c r="B135" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C135" s="13" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7448,7 +7489,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7459,7 +7500,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>
@@ -8540,6 +8581,7 @@
     <mergeCell ref="E140:F140"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -8988,6 +9030,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8995,8 +9038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26B373C-9E20-4F45-A0BB-5F6B2C4A42DF}">
   <dimension ref="A1:A237"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9701,5 +9744,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Formulas done!!!! Now match variables in a list and define paramters and initial values.
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6091AE-EE47-5046-B1DE-D53C164C1A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E79708-2EB8-164E-B3D8-772C3CA29356}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17820" yWindow="740" windowWidth="12420" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="914">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="916">
   <si>
     <t>wfcreate berlin u 1 200</t>
   </si>
@@ -2398,9 +2398,6 @@
     <t>p_e</t>
   </si>
   <si>
-    <t>Vc</t>
-  </si>
-  <si>
     <t>yc</t>
   </si>
   <si>
@@ -2419,9 +2416,6 @@
     <t>HPc</t>
   </si>
   <si>
-    <t>Bc</t>
-  </si>
-  <si>
     <t>Hc</t>
   </si>
   <si>
@@ -2795,13 +2789,25 @@
   </si>
   <si>
     <t>spread1</t>
+  </si>
+  <si>
+    <t>CGeK_E</t>
+  </si>
+  <si>
+    <t>cgh1_e</t>
+  </si>
+  <si>
+    <t>infle</t>
+  </si>
+  <si>
+    <t>V1K_E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2849,6 +2855,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3075,7 +3088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3135,6 +3148,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3228,9 +3243,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59908B7B-EBC3-344F-9113-3BA63F6E78FB}" name="Tabelle1" displayName="Tabelle1" ref="A1:D138" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}"/>
+  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Capitalists"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
-    <sortCondition ref="B1:B138"/>
+    <sortCondition ref="A1:A138"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{7F596A33-4614-6C40-BB1D-09C449AA6172}" name="Number" dataDxfId="2"/>
@@ -3541,7 +3562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A2193-852C-D841-9B05-41DA338A33B9}">
   <dimension ref="A2:A482"/>
   <sheetViews>
-    <sheetView topLeftCell="A361" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A244" sqref="A244"/>
     </sheetView>
   </sheetViews>
@@ -5950,10 +5971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
-  <dimension ref="A1:F321"/>
+  <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C106" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="C149" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E168" sqref="E168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5983,10 +6004,10 @@
         <v>751</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -5997,238 +6018,238 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="46">
+        <v>4</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>5</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>9</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>32</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>745</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>33</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>745</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>457</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>37</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>745</v>
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>41</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>745</v>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>42</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>745</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="46">
+        <v>8</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>876</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>745</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>51</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>745</v>
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>743</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>52</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>745</v>
+        <v>434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>53</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>745</v>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="46">
+        <v>12</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>876</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>477</v>
+        <v>436</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>67</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>745</v>
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>90</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>745</v>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>91</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>745</v>
+        <v>438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>113</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>745</v>
+        <v>439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="46">
+        <v>16</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>876</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11">
-        <v>120</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>745</v>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="46">
+        <v>17</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>876</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>894</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11">
-        <v>121</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>745</v>
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>38</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>745</v>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>462</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>39</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>745</v>
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>40</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>745</v>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>112</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>745</v>
+        <v>445</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6239,7 +6260,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6250,1235 +6271,1235 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
-        <v>99</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>422</v>
+    <row r="26" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>743</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9">
-        <v>103</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>422</v>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>26</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9">
-        <v>106</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>422</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>27</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9">
-        <v>114</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>422</v>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>28</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>535</v>
-      </c>
-      <c r="D29" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9">
-        <v>115</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>422</v>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>29</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>536</v>
+        <v>453</v>
       </c>
       <c r="D30" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9">
-        <v>116</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>422</v>
+        <v>878</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>30</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>537</v>
+        <v>454</v>
       </c>
       <c r="D31" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9">
-        <v>123</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>422</v>
+        <v>879</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>31</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9">
-        <v>124</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C33" s="23" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9">
-        <v>125</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>753</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9">
-        <v>126</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>422</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>752</v>
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9">
-        <v>127</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>422</v>
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>424</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5">
-        <v>6</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>424</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>421</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
-        <v>13</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>424</v>
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="5">
-        <v>18</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>424</v>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
-        <v>20</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>424</v>
+        <v>462</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="5">
-        <v>34</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>424</v>
+        <v>463</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
-        <v>35</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>424</v>
+        <v>464</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="5">
-        <v>43</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>424</v>
+        <v>465</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>745</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>424</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="5">
-        <v>61</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>424</v>
+        <v>467</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="10">
+        <v>44</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
-        <v>68</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>424</v>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="10">
+        <v>45</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>424</v>
       </c>
       <c r="C47" s="13" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="10">
+        <v>47</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10">
+        <v>48</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8">
+        <v>49</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="7">
+        <v>54</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="7">
+        <v>55</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>56</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>57</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="7">
+        <v>58</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="8">
+        <v>59</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="46">
+        <v>60</v>
+      </c>
+      <c r="B61" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="46">
+        <v>63</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="8">
+        <v>64</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="8">
+        <v>65</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7">
+        <v>66</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>69</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C71" s="13" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
-        <v>93</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="5">
-        <v>94</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
-        <v>95</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="5">
-        <v>96</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="5">
-        <v>100</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="5">
-        <v>107</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
-        <v>108</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="5">
-        <v>109</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="5">
-        <v>117</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="10">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="10">
         <v>72</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10">
-        <v>73</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="10">
-        <v>74</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C59" s="13" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="10">
-        <v>75</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="10">
-        <v>76</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="10">
-        <v>77</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="10">
-        <v>78</v>
-      </c>
-      <c r="B63" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="10">
-        <v>79</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C64" s="13" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="10">
-        <v>80</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="10">
-        <v>81</v>
-      </c>
-      <c r="B66" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10">
-        <v>82</v>
-      </c>
-      <c r="B67" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="10">
-        <v>83</v>
-      </c>
-      <c r="B68" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="10">
-        <v>84</v>
-      </c>
-      <c r="B69" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C69" s="13" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="10">
-        <v>85</v>
-      </c>
-      <c r="B70" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="10">
-        <v>86</v>
-      </c>
-      <c r="B71" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="10">
-        <v>87</v>
-      </c>
-      <c r="B72" s="20" t="s">
-        <v>746</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="10">
-        <v>88</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C73" s="13" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C74" s="13" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C75" s="13" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="10">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="46">
-        <v>118</v>
-      </c>
-      <c r="B81" s="47" t="s">
-        <v>878</v>
+        <v>501</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
+        <v>80</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>746</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10">
-        <v>119</v>
+        <v>81</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>746</v>
       </c>
       <c r="C82" s="13" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="10">
+        <v>82</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="10">
+        <v>83</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C84" s="13" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="10">
+        <v>84</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C85" s="13" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="10">
+        <v>85</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="10">
+        <v>86</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="10">
+        <v>87</v>
+      </c>
+      <c r="B88" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="10">
+        <v>88</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C89" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="10">
+        <v>89</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>90</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>91</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="7">
+        <v>92</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>743</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C95" s="13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C97" s="13" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="6">
+        <v>98</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C98" s="13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="9">
+        <v>99</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C99" s="13" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="5">
+        <v>100</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C100" s="13" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="6">
+        <v>101</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C101" s="13" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="46">
+        <v>102</v>
+      </c>
+      <c r="B102" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="C102" s="13" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="9">
+        <v>103</v>
+      </c>
+      <c r="B103" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C103" s="13" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="8">
+        <v>104</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C104" s="13" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="8">
+        <v>105</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="9">
+        <v>106</v>
+      </c>
+      <c r="B106" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="5">
+        <v>107</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="5">
+        <v>108</v>
+      </c>
+      <c r="B108" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="5">
+        <v>109</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="10">
+        <v>110</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="10">
+        <v>111</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="C111" s="13" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="4">
+        <v>112</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C112" s="13" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="4">
+        <v>113</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>745</v>
+      </c>
+      <c r="C113" s="13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="9">
+        <v>114</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C114" s="13" t="s">
+        <v>535</v>
+      </c>
+      <c r="D114" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="9">
+        <v>115</v>
+      </c>
+      <c r="B115" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C115" s="13" t="s">
+        <v>536</v>
+      </c>
+      <c r="D115" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="9">
+        <v>116</v>
+      </c>
+      <c r="B116" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C116" s="13" t="s">
+        <v>537</v>
+      </c>
+      <c r="D116" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="5">
+        <v>117</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C117" s="13" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="46">
+        <v>118</v>
+      </c>
+      <c r="B118" s="47" t="s">
+        <v>876</v>
+      </c>
+      <c r="C118" s="13" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="10">
+        <v>119</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>422</v>
+      </c>
+      <c r="C119" s="13" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="8">
-        <v>11</v>
-      </c>
-      <c r="B83" s="18" t="s">
+    <row r="120" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="11">
+        <v>120</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="11">
+        <v>121</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="8">
+        <v>122</v>
+      </c>
+      <c r="B122" s="18" t="s">
         <v>423</v>
       </c>
-      <c r="C83" s="13" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="8">
-        <v>22</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="8">
-        <v>26</v>
-      </c>
-      <c r="B85" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="8">
-        <v>27</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="8">
-        <v>28</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="8">
-        <v>29</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>453</v>
-      </c>
-      <c r="D88" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="8">
-        <v>30</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C89" s="13" t="s">
-        <v>454</v>
-      </c>
-      <c r="D89" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="8">
-        <v>31</v>
-      </c>
-      <c r="B90" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C90" s="13" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="8">
-        <v>49</v>
-      </c>
-      <c r="B91" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="8">
-        <v>59</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="8">
-        <v>64</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="8">
-        <v>65</v>
-      </c>
-      <c r="B94" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="8">
-        <v>104</v>
-      </c>
-      <c r="B95" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C95" s="13" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="8">
-        <v>105</v>
-      </c>
-      <c r="B96" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="8">
-        <v>122</v>
-      </c>
-      <c r="B97" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="C97" s="13" t="s">
+      <c r="C122" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="D97" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="7">
-        <v>10</v>
-      </c>
-      <c r="B98" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C98" s="13" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="7">
-        <v>25</v>
-      </c>
-      <c r="B99" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C99" s="13" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="7">
-        <v>54</v>
-      </c>
-      <c r="B100" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="7">
-        <v>55</v>
-      </c>
-      <c r="B101" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="7">
-        <v>56</v>
-      </c>
-      <c r="B102" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="7">
-        <v>57</v>
-      </c>
-      <c r="B103" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="7">
-        <v>58</v>
-      </c>
-      <c r="B104" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="7">
-        <v>66</v>
-      </c>
-      <c r="B105" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C105" s="13" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="7">
-        <v>92</v>
-      </c>
-      <c r="B106" s="17" t="s">
-        <v>743</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="12">
-        <v>129</v>
-      </c>
-      <c r="B107" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="12">
-        <v>130</v>
-      </c>
-      <c r="B108" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="12">
-        <v>131</v>
-      </c>
-      <c r="B109" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="12">
-        <v>132</v>
-      </c>
-      <c r="B110" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="12">
-        <v>133</v>
-      </c>
-      <c r="B111" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="12">
-        <v>134</v>
-      </c>
-      <c r="B112" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="12">
-        <v>135</v>
-      </c>
-      <c r="B113" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C113" s="13" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="12">
-        <v>2</v>
-      </c>
-      <c r="B114" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C114" s="13" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="12">
-        <v>3</v>
-      </c>
-      <c r="B115" s="22" t="s">
-        <v>744</v>
-      </c>
-      <c r="C115" s="13" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="46">
-        <v>4</v>
-      </c>
-      <c r="B116" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C116" s="13" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="46">
-        <v>8</v>
-      </c>
-      <c r="B117" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C117" s="13" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="46">
-        <v>12</v>
-      </c>
-      <c r="B118" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C118" s="13" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="46">
-        <v>16</v>
-      </c>
-      <c r="B119" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="46">
-        <v>17</v>
-      </c>
-      <c r="B120" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C120" s="13" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="46">
-        <v>60</v>
-      </c>
-      <c r="B121" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C121" s="23" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="46">
-        <v>63</v>
-      </c>
-      <c r="B122" s="47" t="s">
-        <v>878</v>
-      </c>
-      <c r="C122" s="13" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="46">
-        <v>102</v>
-      </c>
-      <c r="B123" s="47" t="s">
-        <v>878</v>
+      <c r="D122" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="9">
+        <v>123</v>
+      </c>
+      <c r="B123" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="6">
-        <v>7</v>
-      </c>
-      <c r="B124" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C124" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="6">
-        <v>14</v>
-      </c>
-      <c r="B125" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C125" s="13" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="6">
-        <v>15</v>
-      </c>
-      <c r="B126" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C126" s="13" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="6">
-        <v>19</v>
-      </c>
-      <c r="B127" s="16" t="s">
-        <v>421</v>
+        <v>542</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="9">
+        <v>124</v>
+      </c>
+      <c r="B124" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C124" s="52" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="9">
+        <v>125</v>
+      </c>
+      <c r="B125" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C125" s="52" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="9">
+        <v>126</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>422</v>
+      </c>
+      <c r="C126" s="51" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="9">
+        <v>127</v>
+      </c>
+      <c r="B127" s="19" t="s">
+        <v>422</v>
       </c>
       <c r="C127" s="13" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="B128" s="16" t="s">
         <v>421</v>
       </c>
       <c r="C128" s="13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="6">
-        <v>36</v>
-      </c>
-      <c r="B129" s="16" t="s">
-        <v>421</v>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="12">
+        <v>129</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C129" s="13" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="6">
-        <v>62</v>
-      </c>
-      <c r="B130" s="16" t="s">
-        <v>421</v>
-      </c>
-      <c r="C130" s="45" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="6">
-        <v>69</v>
-      </c>
-      <c r="B131" s="16" t="s">
-        <v>421</v>
+        <v>545</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="12">
+        <v>130</v>
+      </c>
+      <c r="B130" s="22" t="s">
+        <v>744</v>
+      </c>
+      <c r="C130" s="13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="12">
+        <v>131</v>
+      </c>
+      <c r="B131" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C131" s="13" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="6">
-        <v>71</v>
-      </c>
-      <c r="B132" s="16" t="s">
-        <v>421</v>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="12">
+        <v>132</v>
+      </c>
+      <c r="B132" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C132" s="13" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="6">
-        <v>98</v>
-      </c>
-      <c r="B133" s="16" t="s">
-        <v>421</v>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="12">
+        <v>133</v>
+      </c>
+      <c r="B133" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C133" s="13" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="6">
-        <v>101</v>
-      </c>
-      <c r="B134" s="16" t="s">
-        <v>421</v>
+        <v>549</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="12">
+        <v>134</v>
+      </c>
+      <c r="B134" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C134" s="13" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="6">
-        <v>128</v>
-      </c>
-      <c r="B135" s="16" t="s">
-        <v>421</v>
+        <v>550</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="12">
+        <v>135</v>
+      </c>
+      <c r="B135" s="22" t="s">
+        <v>744</v>
       </c>
       <c r="C135" s="13" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7489,7 +7510,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7500,7 +7521,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>
@@ -7528,7 +7549,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E142" s="42" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="F142" s="42" t="s">
         <v>759</v>
@@ -7536,7 +7557,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E143" s="41" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F143" s="41" t="s">
         <v>760</v>
@@ -7544,7 +7565,7 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E144" s="41" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="F144" s="41" t="s">
         <v>761</v>
@@ -7600,7 +7621,7 @@
     </row>
     <row r="151" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E151" s="41" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="F151" s="41" t="s">
         <v>768</v>
@@ -7608,7 +7629,7 @@
     </row>
     <row r="152" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E152" s="41" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F152" s="41" t="s">
         <v>769</v>
@@ -7616,7 +7637,7 @@
     </row>
     <row r="153" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E153" s="41" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F153" s="41" t="s">
         <v>770</v>
@@ -7624,7 +7645,7 @@
     </row>
     <row r="154" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E154" s="41" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F154" s="41" t="s">
         <v>771</v>
@@ -7640,7 +7661,7 @@
     </row>
     <row r="156" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E156" s="41" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F156" s="41" t="s">
         <v>773</v>
@@ -7648,15 +7669,15 @@
     </row>
     <row r="157" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E157" s="41" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="F157" s="41" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="158" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E158" s="41" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="F158" s="41" t="s">
         <v>776</v>
@@ -7664,7 +7685,7 @@
     </row>
     <row r="159" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E159" s="41" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F159" s="41" t="s">
         <v>775</v>
@@ -7672,410 +7693,420 @@
     </row>
     <row r="160" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E160" s="41" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F160" s="41" t="s">
         <v>777</v>
       </c>
     </row>
     <row r="161" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E161" s="43"/>
+      <c r="E161" s="43" t="s">
+        <v>912</v>
+      </c>
       <c r="F161" s="43" t="s">
         <v>778</v>
       </c>
     </row>
     <row r="162" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E162" s="43"/>
+      <c r="E162" s="43" t="s">
+        <v>913</v>
+      </c>
       <c r="F162" s="43" t="s">
         <v>779</v>
       </c>
     </row>
     <row r="163" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E163" s="43"/>
+      <c r="E163" s="43" t="s">
+        <v>914</v>
+      </c>
       <c r="F163" s="43" t="s">
         <v>780</v>
       </c>
     </row>
     <row r="164" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E164" s="41" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F164" s="41" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
     </row>
     <row r="165" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E165" s="41" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="F165" s="41" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="166" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E166" s="41" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F166" s="41" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="167" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E167" s="41" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F167" s="41" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="168" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E168" s="41" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F168" s="41" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="169" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E169" s="41" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="F169" s="41" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="170" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E170" s="41" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F170" s="41" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="171" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E171" s="41"/>
       <c r="F171" s="41" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="172" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E172" s="41"/>
+      <c r="E172" s="41" t="s">
+        <v>848</v>
+      </c>
       <c r="F172" s="41" t="s">
-        <v>789</v>
+        <v>767</v>
       </c>
     </row>
     <row r="173" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E173" s="41" t="s">
-        <v>850</v>
+        <v>915</v>
       </c>
       <c r="F173" s="41" t="s">
-        <v>767</v>
+        <v>788</v>
       </c>
     </row>
     <row r="174" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E174" s="41"/>
+      <c r="E174" s="41" t="s">
+        <v>834</v>
+      </c>
       <c r="F174" s="41" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="175" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E175" s="41" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F175" s="41" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="176" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E176" s="41" t="s">
-        <v>837</v>
+        <v>823</v>
       </c>
       <c r="F176" s="41" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="177" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E177" s="41" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F177" s="41" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="178" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E178" s="41" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F178" s="41" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="179" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E179" s="41" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F179" s="41" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="180" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E180" s="41"/>
+      <c r="F180" s="41" t="s">
         <v>795</v>
-      </c>
-    </row>
-    <row r="180" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E180" s="41" t="s">
-        <v>828</v>
-      </c>
-      <c r="F180" s="41" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="181" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E181" s="41"/>
       <c r="F181" s="41" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="182" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E182" s="41"/>
       <c r="F182" s="41" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="183" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E183" s="41"/>
       <c r="F183" s="41" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="184" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E184" s="41"/>
       <c r="F184" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="185" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E185" s="41" t="s">
+        <v>842</v>
+      </c>
+      <c r="F185" s="41" t="s">
         <v>800</v>
-      </c>
-    </row>
-    <row r="185" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E185" s="41"/>
-      <c r="F185" s="41" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="186" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E186" s="41" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F186" s="41" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="187" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E187" s="41" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F187" s="41" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="188" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E188" s="41" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F188" s="41" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="189" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E189" s="41" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F189" s="41" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="190" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E190" s="41" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F190" s="41" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="191" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E191" s="41" t="s">
-        <v>849</v>
-      </c>
+      <c r="E191" s="41"/>
       <c r="F191" s="41" t="s">
-        <v>807</v>
+        <v>762</v>
       </c>
     </row>
     <row r="192" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E192" s="41"/>
       <c r="F192" s="41" t="s">
-        <v>762</v>
+        <v>806</v>
       </c>
     </row>
     <row r="193" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E193" s="41"/>
       <c r="F193" s="41" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="194" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E194" s="41"/>
       <c r="F194" s="41" t="s">
-        <v>809</v>
+        <v>827</v>
       </c>
     </row>
     <row r="195" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E195" s="41"/>
+      <c r="E195" s="41" t="s">
+        <v>836</v>
+      </c>
       <c r="F195" s="41" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="196" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E196" s="41" t="s">
+        <v>837</v>
+      </c>
+      <c r="F196" s="41" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="197" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E197" s="44" t="s">
         <v>838</v>
       </c>
-      <c r="F196" s="41" t="s">
+      <c r="F197" s="41" t="s">
         <v>830</v>
-      </c>
-    </row>
-    <row r="197" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E197" s="41" t="s">
-        <v>839</v>
-      </c>
-      <c r="F197" s="41" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="198" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E198" s="44" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F198" s="41" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="199" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E199" s="44" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F199" s="41" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="200" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E200" s="44" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F200" s="41" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="201" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E201" s="44" t="s">
-        <v>843</v>
+        <v>850</v>
       </c>
       <c r="F201" s="41" t="s">
-        <v>835</v>
+        <v>866</v>
       </c>
     </row>
     <row r="202" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E202" s="44" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F202" s="41" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
     </row>
     <row r="203" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E203" s="44" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F203" s="41" t="s">
-        <v>867</v>
+        <v>858</v>
       </c>
     </row>
     <row r="204" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E204" s="44" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F204" s="41" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="205" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E205" s="44" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F205" s="41" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="206" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E206" s="44" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F206" s="41" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="207" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E207" s="44" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F207" s="41" t="s">
-        <v>863</v>
+        <v>897</v>
       </c>
     </row>
     <row r="208" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E208" s="44" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F208" s="41" t="s">
-        <v>899</v>
+        <v>862</v>
       </c>
     </row>
     <row r="209" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E209" s="44" t="s">
-        <v>859</v>
+        <v>863</v>
       </c>
       <c r="F209" s="41" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
     </row>
     <row r="210" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E210" s="44" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="F210" s="41" t="s">
-        <v>869</v>
+        <v>896</v>
       </c>
     </row>
     <row r="211" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E211" s="44" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="F211" s="41" t="s">
-        <v>898</v>
+        <v>869</v>
       </c>
     </row>
     <row r="212" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E212" s="44" t="s">
+      <c r="E212" s="44"/>
+      <c r="F212" s="41" t="s">
         <v>870</v>
       </c>
-      <c r="F212" s="41" t="s">
+    </row>
+    <row r="213" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E213" s="41" t="s">
         <v>871</v>
       </c>
-    </row>
-    <row r="213" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E213" s="44"/>
       <c r="F213" s="41" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="214" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E214" s="41" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F214" s="41" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
     </row>
     <row r="215" spans="5:6" x14ac:dyDescent="0.2">
@@ -8083,44 +8114,44 @@
         <v>874</v>
       </c>
       <c r="F215" s="41" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="216" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E216" s="41" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="F216" s="41" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
     </row>
     <row r="217" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E217" s="41" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F217" s="41" t="s">
-        <v>872</v>
+        <v>890</v>
       </c>
     </row>
     <row r="218" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E218" s="41" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F218" s="41" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="219" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E219" s="41" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F219" s="41" t="s">
-        <v>893</v>
+        <v>897</v>
       </c>
     </row>
     <row r="220" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E220" s="41" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F220" s="41" t="s">
         <v>899</v>
@@ -8128,69 +8159,69 @@
     </row>
     <row r="221" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E221" s="41" t="s">
-        <v>886</v>
+        <v>871</v>
       </c>
       <c r="F221" s="41" t="s">
-        <v>901</v>
+        <v>873</v>
       </c>
     </row>
     <row r="222" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E222" s="41" t="s">
-        <v>873</v>
+        <v>886</v>
       </c>
       <c r="F222" s="41" t="s">
-        <v>875</v>
+        <v>894</v>
       </c>
     </row>
     <row r="223" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E223" s="41" t="s">
-        <v>888</v>
+        <v>895</v>
       </c>
       <c r="F223" s="41" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
     </row>
     <row r="224" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E224" s="41" t="s">
-        <v>897</v>
+        <v>887</v>
       </c>
       <c r="F224" s="41" t="s">
-        <v>900</v>
+        <v>774</v>
       </c>
     </row>
     <row r="225" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E225" s="41" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="F225" s="41" t="s">
-        <v>774</v>
+        <v>787</v>
       </c>
     </row>
     <row r="226" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E226" s="41" t="s">
-        <v>890</v>
-      </c>
-      <c r="F226" s="41" t="s">
-        <v>789</v>
-      </c>
+        <v>900</v>
+      </c>
+      <c r="F226" s="41"/>
     </row>
     <row r="227" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E227" s="41" t="s">
-        <v>902</v>
-      </c>
-      <c r="F227" s="41"/>
+        <v>901</v>
+      </c>
+      <c r="F227" s="41" t="s">
+        <v>901</v>
+      </c>
     </row>
     <row r="228" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E228" s="41" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F228" s="41" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="229" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E229" s="41" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F229" s="41" t="s">
         <v>904</v>
@@ -8201,24 +8232,20 @@
         <v>905</v>
       </c>
       <c r="F230" s="41" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="231" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E231" s="41" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="F231" s="41" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="232" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E232" s="41" t="s">
-        <v>908</v>
-      </c>
-      <c r="F232" s="41" t="s">
-        <v>909</v>
-      </c>
+      <c r="E232" s="41"/>
+      <c r="F232" s="41"/>
     </row>
     <row r="233" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E233" s="41"/>
@@ -8571,10 +8598,6 @@
     <row r="320" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E320" s="41"/>
       <c r="F320" s="41"/>
-    </row>
-    <row r="321" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E321" s="41"/>
-      <c r="F321" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8592,7 +8615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF9BF1B-431C-9C4E-97D3-85B33ADD80FB}">
   <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A60" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -9038,7 +9061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26B373C-9E20-4F45-A0BB-5F6B2C4A42DF}">
   <dimension ref="A1:A237"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some minor mistakes found. Also variable matching!
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E79708-2EB8-164E-B3D8-772C3CA29356}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3415A677-0DC3-6344-8DDC-5035BBDBC11F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17820" yWindow="740" windowWidth="12420" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="15600" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zezza import" sheetId="1" r:id="rId1"/>
@@ -3139,6 +3139,8 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3148,8 +3150,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -3246,7 +3246,7 @@
   <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Capitalists"/>
+        <filter val="Workers"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -3562,7 +3562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A2193-852C-D841-9B05-41DA338A33B9}">
   <dimension ref="A2:A482"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A88" zoomScale="157" workbookViewId="0">
       <selection activeCell="A244" sqref="A244"/>
     </sheetView>
   </sheetViews>
@@ -5793,16 +5793,16 @@
   <sheetData>
     <row r="1" spans="2:10" ht="26" x14ac:dyDescent="0.3">
       <c r="B1" s="26"/>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="50" t="s">
         <v>420</v>
       </c>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
@@ -5973,8 +5973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C149" zoomScale="141" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E168" sqref="E168"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6062,7 +6062,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6096,11 +6096,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>745</v>
+      <c r="B10" s="18" t="s">
+        <v>423</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>433</v>
@@ -6139,7 +6139,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -6508,7 +6508,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -6673,7 +6673,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -7025,7 +7025,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -7047,7 +7047,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -7058,7 +7058,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>98</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>100</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>101</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>107</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>108</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>109</v>
       </c>
@@ -7287,7 +7287,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>117</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>119</v>
       </c>
       <c r="B119" s="20" t="s">
-        <v>422</v>
+        <v>746</v>
       </c>
       <c r="C119" s="13" t="s">
         <v>540</v>
@@ -7374,7 +7374,7 @@
       <c r="B124" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="C124" s="52" t="s">
+      <c r="C124" s="49" t="s">
         <v>754</v>
       </c>
     </row>
@@ -7385,7 +7385,7 @@
       <c r="B125" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="C125" s="52" t="s">
+      <c r="C125" s="49" t="s">
         <v>753</v>
       </c>
     </row>
@@ -7396,7 +7396,7 @@
       <c r="B126" s="19" t="s">
         <v>422</v>
       </c>
-      <c r="C126" s="51" t="s">
+      <c r="C126" s="48" t="s">
         <v>752</v>
       </c>
     </row>
@@ -7411,7 +7411,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>128</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7521,7 +7521,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>
@@ -7534,10 +7534,10 @@
     </row>
     <row r="139" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="140" spans="1:6" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E140" s="49" t="s">
+      <c r="E140" s="51" t="s">
         <v>756</v>
       </c>
-      <c r="F140" s="50"/>
+      <c r="F140" s="52"/>
     </row>
     <row r="141" spans="1:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E141" s="2" t="s">
@@ -8615,7 +8615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF9BF1B-431C-9C4E-97D3-85B33ADD80FB}">
   <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
+    <sheetView topLeftCell="A77" zoomScale="150" workbookViewId="0">
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -9061,8 +9061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26B373C-9E20-4F45-A0BB-5F6B2C4A42DF}">
   <dimension ref="A1:A237"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView topLeftCell="A63" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
All parameter variables and so on are now matched
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3415A677-0DC3-6344-8DDC-5035BBDBC11F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA18283-EF1D-E446-B640-AA10250B9658}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="15600" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
+    <workbookView xWindow="15240" yWindow="740" windowWidth="15000" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zezza import" sheetId="1" r:id="rId1"/>
@@ -3246,7 +3246,7 @@
   <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Workers"/>
+        <filter val="Expectations"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5973,8 +5973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A45:A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6073,7 +6073,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6227,7 +6227,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -6486,7 +6486,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -6519,7 +6519,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -6761,7 +6761,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -6783,7 +6783,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
         <v>72</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>73</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>74</v>
       </c>
@@ -6827,7 +6827,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
         <v>75</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>76</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>77</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="10">
         <v>78</v>
       </c>
@@ -6871,7 +6871,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10">
         <v>79</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="10">
         <v>80</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10">
         <v>81</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="10">
         <v>82</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="10">
         <v>83</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="10">
         <v>84</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="10">
         <v>85</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="10">
         <v>86</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="10">
         <v>87</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="10">
         <v>88</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="10">
         <v>89</v>
       </c>
@@ -7069,7 +7069,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>98</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>101</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>109</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="10">
         <v>110</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="10">
         <v>111</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="10">
         <v>119</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>128</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7521,7 +7521,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
some parameter in the model. Still figuring stuff out
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA18283-EF1D-E446-B640-AA10250B9658}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4997CCF3-91D4-8240-955B-0693D3FB63E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="740" windowWidth="15000" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
+    <workbookView xWindow="15240" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zezza import" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="916">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="919">
   <si>
     <t>wfcreate berlin u 1 200</t>
   </si>
@@ -2801,6 +2801,15 @@
   </si>
   <si>
     <t>V1K_E</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parameters in asset demand function</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parameters for wage adj function</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Banks spreads on central bank interest rate</t>
   </si>
 </sst>
 </file>
@@ -3243,13 +3252,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59908B7B-EBC3-344F-9113-3BA63F6E78FB}" name="Tabelle1" displayName="Tabelle1" ref="A1:D138" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Expectations"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
     <sortCondition ref="A1:A138"/>
   </sortState>
@@ -3562,8 +3565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A2193-852C-D841-9B05-41DA338A33B9}">
   <dimension ref="A2:A482"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="157" workbookViewId="0">
+      <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3807,8 +3810,8 @@
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>47</v>
+      <c r="A50" s="1" t="s">
+        <v>916</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
@@ -3902,8 +3905,8 @@
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>66</v>
+      <c r="A70" s="1" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
@@ -3957,8 +3960,8 @@
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>77</v>
+      <c r="A83" s="1" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
@@ -5973,8 +5976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="158" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A46" sqref="A45:A46"/>
+    <sheetView topLeftCell="A69" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6007,7 +6010,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6018,7 +6021,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6029,7 +6032,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6040,7 +6043,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -6051,7 +6054,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6062,7 +6065,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6073,7 +6076,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6084,7 +6087,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="46">
         <v>8</v>
       </c>
@@ -6095,7 +6098,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -6106,7 +6109,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -6117,7 +6120,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -6128,7 +6131,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46">
         <v>12</v>
       </c>
@@ -6139,7 +6142,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6150,7 +6153,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6172,7 +6175,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46">
         <v>16</v>
       </c>
@@ -6183,7 +6186,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46">
         <v>17</v>
       </c>
@@ -6194,7 +6197,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6205,7 +6208,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6216,7 +6219,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6227,7 +6230,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6238,7 +6241,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -6249,7 +6252,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6260,7 +6263,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -6282,7 +6285,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -6293,7 +6296,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -6304,7 +6307,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -6315,7 +6318,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -6329,7 +6332,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -6343,7 +6346,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -6354,7 +6357,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -6365,7 +6368,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -6376,7 +6379,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6387,7 +6390,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6398,7 +6401,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -6409,7 +6412,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -6420,7 +6423,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -6431,7 +6434,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -6442,7 +6445,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -6453,7 +6456,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -6464,7 +6467,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -6475,7 +6478,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -6508,7 +6511,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -6541,7 +6544,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -6552,7 +6555,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -6563,7 +6566,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -6574,7 +6577,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -6585,7 +6588,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -6596,7 +6599,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -6607,7 +6610,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -6618,7 +6621,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -6629,7 +6632,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -6640,7 +6643,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -6651,7 +6654,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -6662,7 +6665,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="46">
         <v>60</v>
       </c>
@@ -6673,7 +6676,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6684,7 +6687,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -6695,7 +6698,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="46">
         <v>63</v>
       </c>
@@ -6706,7 +6709,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -6717,7 +6720,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -6728,7 +6731,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -6739,7 +6742,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -6750,7 +6753,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6761,7 +6764,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -6772,7 +6775,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6783,7 +6786,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -6992,7 +6995,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -7003,7 +7006,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -7014,7 +7017,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -7025,7 +7028,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -7036,7 +7039,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -7047,7 +7050,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -7058,7 +7061,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -7069,7 +7072,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>98</v>
       </c>
@@ -7080,7 +7083,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>99</v>
       </c>
@@ -7091,7 +7094,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>100</v>
       </c>
@@ -7102,7 +7105,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>101</v>
       </c>
@@ -7113,7 +7116,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="46">
         <v>102</v>
       </c>
@@ -7124,7 +7127,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>103</v>
       </c>
@@ -7135,7 +7138,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>104</v>
       </c>
@@ -7146,7 +7149,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>105</v>
       </c>
@@ -7157,7 +7160,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>106</v>
       </c>
@@ -7168,7 +7171,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>107</v>
       </c>
@@ -7179,7 +7182,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>108</v>
       </c>
@@ -7190,7 +7193,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>109</v>
       </c>
@@ -7223,7 +7226,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>112</v>
       </c>
@@ -7234,7 +7237,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>113</v>
       </c>
@@ -7245,7 +7248,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="9">
         <v>114</v>
       </c>
@@ -7259,7 +7262,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9">
         <v>115</v>
       </c>
@@ -7273,7 +7276,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9">
         <v>116</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>117</v>
       </c>
@@ -7298,7 +7301,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="46">
         <v>118</v>
       </c>
@@ -7320,7 +7323,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="11">
         <v>120</v>
       </c>
@@ -7331,7 +7334,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="11">
         <v>121</v>
       </c>
@@ -7342,7 +7345,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <v>122</v>
       </c>
@@ -7356,7 +7359,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9">
         <v>123</v>
       </c>
@@ -7367,7 +7370,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="9">
         <v>124</v>
       </c>
@@ -7378,7 +7381,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>125</v>
       </c>
@@ -7389,7 +7392,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9">
         <v>126</v>
       </c>
@@ -7400,7 +7403,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9">
         <v>127</v>
       </c>
@@ -7411,7 +7414,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>128</v>
       </c>
@@ -7422,7 +7425,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="12">
         <v>129</v>
       </c>
@@ -7433,7 +7436,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="12">
         <v>130</v>
       </c>
@@ -7444,7 +7447,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="12">
         <v>131</v>
       </c>
@@ -7455,7 +7458,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="12">
         <v>132</v>
       </c>
@@ -7466,7 +7469,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="12">
         <v>133</v>
       </c>
@@ -7477,7 +7480,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="12">
         <v>134</v>
       </c>
@@ -7488,7 +7491,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="12">
         <v>135</v>
       </c>
@@ -7499,7 +7502,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7510,7 +7513,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7521,7 +7524,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Parameter and exogenous so sofar set!
Now initial values!
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4997CCF3-91D4-8240-955B-0693D3FB63E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1B301C-ACBC-BA4E-9C82-C364E45A4E1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15240" yWindow="740" windowWidth="15000" windowHeight="18900" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
+    <workbookView xWindow="15660" yWindow="740" windowWidth="14580" windowHeight="18900" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Zezza import" sheetId="1" r:id="rId1"/>
@@ -3252,7 +3252,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59908B7B-EBC3-344F-9113-3BA63F6E78FB}" name="Tabelle1" displayName="Tabelle1" ref="A1:D138" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}"/>
+  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Workers"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
     <sortCondition ref="A1:A138"/>
   </sortState>
@@ -3565,7 +3571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2A2193-852C-D841-9B05-41DA338A33B9}">
   <dimension ref="A2:A482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="157" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="157" workbookViewId="0">
       <selection activeCell="A193" sqref="A193"/>
     </sheetView>
   </sheetViews>
@@ -5976,8 +5982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6010,7 +6016,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -6021,7 +6027,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6032,7 +6038,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6043,7 +6049,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -6054,7 +6060,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -6065,7 +6071,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6087,7 +6093,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="46">
         <v>8</v>
       </c>
@@ -6098,7 +6104,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -6109,7 +6115,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -6120,7 +6126,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -6131,7 +6137,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46">
         <v>12</v>
       </c>
@@ -6142,7 +6148,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6175,7 +6181,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46">
         <v>16</v>
       </c>
@@ -6186,7 +6192,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46">
         <v>17</v>
       </c>
@@ -6197,7 +6203,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6219,7 +6225,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6241,7 +6247,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -6252,7 +6258,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6263,7 +6269,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6274,7 +6280,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -6285,7 +6291,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -6296,7 +6302,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -6307,7 +6313,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -6318,7 +6324,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -6332,7 +6338,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -6346,7 +6352,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -6357,7 +6363,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -6368,7 +6374,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -6379,7 +6385,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6390,7 +6396,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6412,7 +6418,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -6423,7 +6429,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -6434,7 +6440,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -6445,7 +6451,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -6456,7 +6462,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -6467,7 +6473,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -6478,7 +6484,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -6489,7 +6495,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -6500,7 +6506,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -6511,7 +6517,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -6522,7 +6528,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -6533,7 +6539,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -6544,7 +6550,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -6555,7 +6561,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -6566,7 +6572,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -6577,7 +6583,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -6588,7 +6594,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -6599,7 +6605,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -6610,7 +6616,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -6621,7 +6627,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -6632,7 +6638,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -6643,7 +6649,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -6654,7 +6660,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -6665,7 +6671,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="46">
         <v>60</v>
       </c>
@@ -6676,7 +6682,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6698,7 +6704,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="46">
         <v>63</v>
       </c>
@@ -6709,7 +6715,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -6720,7 +6726,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -6731,7 +6737,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -6742,7 +6748,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -6753,7 +6759,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6775,7 +6781,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6797,7 +6803,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
         <v>72</v>
       </c>
@@ -6808,7 +6814,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>73</v>
       </c>
@@ -6819,7 +6825,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>74</v>
       </c>
@@ -6830,7 +6836,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
         <v>75</v>
       </c>
@@ -6841,7 +6847,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>76</v>
       </c>
@@ -6852,7 +6858,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>77</v>
       </c>
@@ -6863,7 +6869,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="10">
         <v>78</v>
       </c>
@@ -6874,7 +6880,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10">
         <v>79</v>
       </c>
@@ -6885,7 +6891,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="10">
         <v>80</v>
       </c>
@@ -6896,7 +6902,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10">
         <v>81</v>
       </c>
@@ -6907,7 +6913,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="10">
         <v>82</v>
       </c>
@@ -6918,7 +6924,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="10">
         <v>83</v>
       </c>
@@ -6929,7 +6935,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="10">
         <v>84</v>
       </c>
@@ -6940,7 +6946,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="10">
         <v>85</v>
       </c>
@@ -6951,7 +6957,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="10">
         <v>86</v>
       </c>
@@ -6962,7 +6968,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="10">
         <v>87</v>
       </c>
@@ -6973,7 +6979,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="10">
         <v>88</v>
       </c>
@@ -6984,7 +6990,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="10">
         <v>89</v>
       </c>
@@ -6995,7 +7001,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -7006,7 +7012,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -7017,7 +7023,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -7028,7 +7034,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -7039,7 +7045,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -7050,7 +7056,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -7061,7 +7067,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -7083,7 +7089,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>99</v>
       </c>
@@ -7094,7 +7100,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>100</v>
       </c>
@@ -7116,7 +7122,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="46">
         <v>102</v>
       </c>
@@ -7127,7 +7133,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>103</v>
       </c>
@@ -7138,7 +7144,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>104</v>
       </c>
@@ -7149,7 +7155,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>105</v>
       </c>
@@ -7160,7 +7166,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>106</v>
       </c>
@@ -7171,7 +7177,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>107</v>
       </c>
@@ -7182,7 +7188,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>108</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>109</v>
       </c>
@@ -7204,7 +7210,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="10">
         <v>110</v>
       </c>
@@ -7215,7 +7221,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="10">
         <v>111</v>
       </c>
@@ -7226,7 +7232,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4">
         <v>112</v>
       </c>
@@ -7237,7 +7243,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4">
         <v>113</v>
       </c>
@@ -7248,7 +7254,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="9">
         <v>114</v>
       </c>
@@ -7262,7 +7268,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9">
         <v>115</v>
       </c>
@@ -7276,7 +7282,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9">
         <v>116</v>
       </c>
@@ -7290,7 +7296,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>117</v>
       </c>
@@ -7301,7 +7307,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="46">
         <v>118</v>
       </c>
@@ -7312,7 +7318,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="10">
         <v>119</v>
       </c>
@@ -7323,7 +7329,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="11">
         <v>120</v>
       </c>
@@ -7334,7 +7340,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="11">
         <v>121</v>
       </c>
@@ -7345,7 +7351,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <v>122</v>
       </c>
@@ -7359,7 +7365,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9">
         <v>123</v>
       </c>
@@ -7370,7 +7376,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="9">
         <v>124</v>
       </c>
@@ -7381,7 +7387,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>125</v>
       </c>
@@ -7392,7 +7398,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9">
         <v>126</v>
       </c>
@@ -7403,7 +7409,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9">
         <v>127</v>
       </c>
@@ -7425,7 +7431,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="12">
         <v>129</v>
       </c>
@@ -7436,7 +7442,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="12">
         <v>130</v>
       </c>
@@ -7447,7 +7453,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="12">
         <v>131</v>
       </c>
@@ -7458,7 +7464,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="12">
         <v>132</v>
       </c>
@@ -7469,7 +7475,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="12">
         <v>133</v>
       </c>
@@ -7480,7 +7486,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="12">
         <v>134</v>
       </c>
@@ -7491,7 +7497,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="12">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
Model is running! Cyclical and not watertight!!!
</commit_message>
<xml_diff>
--- a/resources/Zezza_model.xlsx
+++ b/resources/Zezza_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandertoplitsch/R-Projects/sfc/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C71ED6E-57E0-6241-B6EE-0B6010DD4F3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96BA790-071D-5E45-BF2A-4C1BDF5E45EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{44A6EE4B-67DD-6848-9F25-F36A67DE2AE3}"/>
   </bookViews>
@@ -3255,14 +3255,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59908B7B-EBC3-344F-9113-3BA63F6E78FB}" name="Tabelle1" displayName="Tabelle1" ref="A1:D138" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="AD, UR, W"/>
-        <filter val="Expectations"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D138" xr:uid="{8E25C6CC-CF7F-994A-A82C-4EAD9E2A3785}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D138">
     <sortCondition ref="A1:A138"/>
   </sortState>
@@ -5986,8 +5979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C20B65-CFC5-B947-B611-B7766DAA33A0}">
   <dimension ref="A1:F320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="216" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="216" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6031,7 +6024,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6042,7 +6035,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6053,7 +6046,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="46">
         <v>4</v>
       </c>
@@ -6075,7 +6068,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -6086,7 +6079,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -6097,7 +6090,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="46">
         <v>8</v>
       </c>
@@ -6108,7 +6101,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -6119,7 +6112,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -6130,7 +6123,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -6141,7 +6134,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46">
         <v>12</v>
       </c>
@@ -6152,7 +6145,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -6163,7 +6156,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -6174,7 +6167,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -6188,7 +6181,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="46">
         <v>16</v>
       </c>
@@ -6199,7 +6192,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46">
         <v>17</v>
       </c>
@@ -6210,7 +6203,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -6221,7 +6214,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -6232,7 +6225,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -6243,7 +6236,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -6254,7 +6247,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>22</v>
       </c>
@@ -6265,7 +6258,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -6276,7 +6269,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -6287,7 +6280,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>25</v>
       </c>
@@ -6298,7 +6291,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>26</v>
       </c>
@@ -6309,7 +6302,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -6320,7 +6313,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>28</v>
       </c>
@@ -6331,7 +6324,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>29</v>
       </c>
@@ -6345,7 +6338,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -6359,7 +6352,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>31</v>
       </c>
@@ -6392,7 +6385,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -6403,7 +6396,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -6414,7 +6407,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>36</v>
       </c>
@@ -6491,7 +6484,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -6524,7 +6517,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -6557,7 +6550,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>49</v>
       </c>
@@ -6612,7 +6605,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7">
         <v>54</v>
       </c>
@@ -6623,7 +6616,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7">
         <v>55</v>
       </c>
@@ -6634,7 +6627,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7">
         <v>56</v>
       </c>
@@ -6645,7 +6638,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7">
         <v>57</v>
       </c>
@@ -6656,7 +6649,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7">
         <v>58</v>
       </c>
@@ -6667,7 +6660,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>59</v>
       </c>
@@ -6678,7 +6671,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="46">
         <v>60</v>
       </c>
@@ -6689,7 +6682,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -6700,7 +6693,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>62</v>
       </c>
@@ -6711,7 +6704,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="46">
         <v>63</v>
       </c>
@@ -6722,7 +6715,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>64</v>
       </c>
@@ -6733,7 +6726,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="8">
         <v>65</v>
       </c>
@@ -6744,7 +6737,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="7">
         <v>66</v>
       </c>
@@ -6766,7 +6759,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="22" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -6777,7 +6770,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>69</v>
       </c>
@@ -6788,7 +6781,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -6799,7 +6792,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -7030,7 +7023,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -7041,7 +7034,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>93</v>
       </c>
@@ -7052,7 +7045,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>94</v>
       </c>
@@ -7063,7 +7056,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>95</v>
       </c>
@@ -7074,7 +7067,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>96</v>
       </c>
@@ -7085,7 +7078,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="98" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>98</v>
       </c>
@@ -7096,7 +7089,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="9">
         <v>99</v>
       </c>
@@ -7107,7 +7100,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>100</v>
       </c>
@@ -7118,7 +7111,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="101" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="6">
         <v>101</v>
       </c>
@@ -7129,7 +7122,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="46">
         <v>102</v>
       </c>
@@ -7140,7 +7133,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="9">
         <v>103</v>
       </c>
@@ -7151,7 +7144,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="8">
         <v>104</v>
       </c>
@@ -7162,7 +7155,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="8">
         <v>105</v>
       </c>
@@ -7173,7 +7166,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="9">
         <v>106</v>
       </c>
@@ -7184,7 +7177,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>107</v>
       </c>
@@ -7195,7 +7188,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>108</v>
       </c>
@@ -7206,7 +7199,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>109</v>
       </c>
@@ -7261,7 +7254,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="9">
         <v>114</v>
       </c>
@@ -7275,7 +7268,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="9">
         <v>115</v>
       </c>
@@ -7289,7 +7282,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="9">
         <v>116</v>
       </c>
@@ -7303,7 +7296,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>117</v>
       </c>
@@ -7314,7 +7307,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="46">
         <v>118</v>
       </c>
@@ -7358,7 +7351,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="8">
         <v>122</v>
       </c>
@@ -7372,7 +7365,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="9">
         <v>123</v>
       </c>
@@ -7383,7 +7376,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="9">
         <v>124</v>
       </c>
@@ -7394,7 +7387,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="9">
         <v>125</v>
       </c>
@@ -7405,7 +7398,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="9">
         <v>126</v>
       </c>
@@ -7416,7 +7409,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="9">
         <v>127</v>
       </c>
@@ -7427,7 +7420,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>128</v>
       </c>
@@ -7438,7 +7431,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="12">
         <v>129</v>
       </c>
@@ -7449,7 +7442,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="12">
         <v>130</v>
       </c>
@@ -7460,7 +7453,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="12">
         <v>131</v>
       </c>
@@ -7471,7 +7464,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="12">
         <v>132</v>
       </c>
@@ -7482,7 +7475,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="12">
         <v>133</v>
       </c>
@@ -7493,7 +7486,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="12">
         <v>134</v>
       </c>
@@ -7504,7 +7497,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="12">
         <v>135</v>
       </c>
@@ -7515,7 +7508,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>136</v>
       </c>
@@ -7526,7 +7519,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="17" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="6">
         <v>137</v>
       </c>
@@ -7537,7 +7530,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>138</v>
       </c>

</xml_diff>